<commit_message>
Updated Master_Script_PRMS.R to fix working directory issues
</commit_message>
<xml_diff>
--- a/Supply/Documentation/RR_PRMS_StationList.xlsx
+++ b/Supply/Documentation/RR_PRMS_StationList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\palemi\Documents\Github\DWRAT_DataScraping\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\palemi\Documents\Github\DWRAT_DataScraping\Supply\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A510BEFD-0C91-45F4-AC6D-4CD8B35BD166}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E2957C5-EEC7-447B-BFB0-ABD2E4FD08A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15750" activeTab="1" xr2:uid="{55E5B8DA-EFB4-40EB-A996-34EBB2C6B909}"/>
+    <workbookView xWindow="34464" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{55E5B8DA-EFB4-40EB-A996-34EBB2C6B909}"/>
   </bookViews>
   <sheets>
     <sheet name="StationList" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="10" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -1785,7 +1785,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="CIMIS" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Station">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="CIMIS" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Station">
   <location ref="D3:D29" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="8">
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
@@ -1961,7 +1961,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{12495159-9906-4108-ABA6-894BC3D5D83C}" name="PivotTable3" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="CNRFC IDs">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{12495159-9906-4108-ABA6-894BC3D5D83C}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="CNRFC IDs">
   <location ref="G1:H15" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField multipleItemSelectionAllowed="1" showAll="0">
@@ -2118,7 +2118,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000001000000}" name="RAWS" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Station">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000001000000}" name="RAWS" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Station">
   <location ref="A4:A12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="8">
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0" defaultSubtotal="0">
@@ -2241,29 +2241,7 @@
   <autoFilter ref="A2:H64" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0">
       <filters>
-        <filter val="CIMIS"/>
         <filter val="DOWNSIZER"/>
-        <filter val="RAWS"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="1">
-      <filters>
-        <filter val="TMAX1"/>
-        <filter val="TMAX2"/>
-        <filter val="TMAX3"/>
-        <filter val="TMAX4"/>
-        <filter val="TMAX5"/>
-        <filter val="TMAX6"/>
-        <filter val="TMAX7"/>
-        <filter val="TMAX8"/>
-        <filter val="TMIN1"/>
-        <filter val="TMIN2"/>
-        <filter val="TMIN3"/>
-        <filter val="TMIN4"/>
-        <filter val="TMIN5"/>
-        <filter val="TMIN6"/>
-        <filter val="TMIN7"/>
-        <filter val="TMIN8"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -2600,8 +2578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B33" sqref="B33:C64"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2672,7 +2650,7 @@
         <v>13537</v>
       </c>
     </row>
-    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -2698,7 +2676,7 @@
         <v>1353</v>
       </c>
     </row>
-    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2750,7 +2728,7 @@
         <v>10188</v>
       </c>
     </row>
-    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -2833,7 +2811,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -2947,7 +2925,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -3056,7 +3034,7 @@
         <v>17716</v>
       </c>
     </row>
-    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -3108,7 +3086,7 @@
         <v>40017</v>
       </c>
     </row>
-    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -3191,7 +3169,7 @@
         <v>11219</v>
       </c>
     </row>
-    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -3243,7 +3221,7 @@
         <v>20020</v>
       </c>
     </row>
-    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -3295,7 +3273,7 @@
         <v>86521</v>
       </c>
     </row>
-    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>8</v>
       </c>
@@ -3495,7 +3473,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>21</v>
       </c>
@@ -3512,7 +3490,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>21</v>
       </c>
@@ -3557,7 +3535,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>21</v>
       </c>
@@ -3574,7 +3552,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>21</v>
       </c>
@@ -3619,7 +3597,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>15</v>
       </c>
@@ -3636,7 +3614,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>15</v>
       </c>
@@ -3761,7 +3739,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>15</v>
       </c>
@@ -3778,7 +3756,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>15</v>
       </c>
@@ -3823,7 +3801,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>15</v>
       </c>
@@ -3854,7 +3832,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>15</v>
       </c>
@@ -3888,8 +3866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCC5C4D8-AB45-4DCC-9F52-27C34EEB0F92}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4113,7 +4091,7 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4463,15 +4441,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F312EB754F236045A0D3EDD082CC91AE" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="241ce865d663be13d7e342f59527821d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b2cf8adb-cf25-47fc-8c92-b53f2a7e7f06" xmlns:ns3="851dfaa3-aae8-4c03-b90c-7dd4a6526d0d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3129014a3b2306d1c4ed4239399361fd" ns2:_="" ns3:_="">
     <xsd:import namespace="b2cf8adb-cf25-47fc-8c92-b53f2a7e7f06"/>
@@ -4648,15 +4617,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEC31F2C-BA94-4757-B459-232C7EAF18FB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2643DE3-C6DD-4C5A-9AE4-EF5AECAB0779}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4673,4 +4643,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEC31F2C-BA94-4757-B459-232C7EAF18FB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>